<commit_message>
Exception handling examples  Day-17
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\KTG\RAJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC8CA12-3E69-47DA-9F05-956435AA8618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB73363-2F59-49D1-A929-02BF936CFC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
   <si>
     <t>Concepts</t>
   </si>
@@ -302,6 +302,12 @@
   </si>
   <si>
     <t>complete pending concepts and revise</t>
+  </si>
+  <si>
+    <t>Day-17</t>
+  </si>
+  <si>
+    <t>exception handling,try ,catch,throw ,throws, finally,user defined exceptions</t>
   </si>
 </sst>
 </file>
@@ -741,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:M166"/>
+  <dimension ref="A3:M167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1081,12 +1087,18 @@
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="D21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="4">
+        <v>44992</v>
+      </c>
       <c r="F21" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" s="5"/>
+        <v>93</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
@@ -1094,40 +1106,40 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="G22" s="5"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="9"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="M23" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
+      <c r="M24" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1137,7 +1149,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -1147,30 +1159,30 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G27" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-      <c r="M27" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
+      <c r="M28" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="3"/>
@@ -1180,7 +1192,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="3"/>
@@ -1190,7 +1202,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="3"/>
@@ -1200,7 +1212,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="3"/>
@@ -1210,7 +1222,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="3"/>
@@ -1219,7 +1231,9 @@
     <row r="34" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
-      <c r="F34" s="3"/>
+      <c r="F34" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="G34" s="10"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -1276,7 +1290,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
+      <c r="G41" s="10"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
@@ -1330,7 +1344,7 @@
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D48" s="6"/>
-      <c r="E48" s="3"/>
+      <c r="E48" s="6"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -1361,6 +1375,7 @@
       <c r="I51" s="3"/>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D52" s="6"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
@@ -2165,10 +2180,17 @@
       <c r="H166" s="3"/>
       <c r="I166" s="3"/>
     </row>
+    <row r="167" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E167" s="3"/>
+      <c r="F167" s="3"/>
+      <c r="G167" s="3"/>
+      <c r="H167" s="3"/>
+      <c r="I167" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="M23" r:id="rId1" xr:uid="{34C8B530-A33E-4B7A-BE11-76AFC55CF670}"/>
+    <hyperlink ref="M24" r:id="rId1" xr:uid="{34C8B530-A33E-4B7A-BE11-76AFC55CF670}"/>
     <hyperlink ref="I9" r:id="rId2" xr:uid="{FD119ECE-9E2E-4E1F-AB4D-5F8FD2F949A4}"/>
     <hyperlink ref="I12" r:id="rId3" xr:uid="{548CAE75-A83E-4759-8D67-8569C4AB1486}"/>
     <hyperlink ref="I3" r:id="rId4" xr:uid="{1D8D861E-CDBB-4089-A57B-B813ECEA241E}"/>

</xml_diff>

<commit_message>
Day-30 Jpa Case study
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\KTG\RAJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34797D99-FFB1-4846-B0E2-A5A72A372ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A043CB-21B9-4146-80A6-253F38A8D12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="126">
   <si>
     <t>Concepts</t>
   </si>
@@ -205,21 +205,6 @@
     <t>case study</t>
   </si>
   <si>
-    <t>css</t>
-  </si>
-  <si>
-    <t>js</t>
-  </si>
-  <si>
-    <t>ts</t>
-  </si>
-  <si>
-    <t>bs</t>
-  </si>
-  <si>
-    <t>angular</t>
-  </si>
-  <si>
     <t>6:35 AM-7:50 AM</t>
   </si>
   <si>
@@ -410,6 +395,15 @@
   </si>
   <si>
     <t>Refer JPQL CRUD</t>
+  </si>
+  <si>
+    <t>jpa case study, maven</t>
+  </si>
+  <si>
+    <t>6:00PM-7:00PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refer employee Crud ,complete student crud using layered architecture </t>
   </si>
 </sst>
 </file>
@@ -852,7 +846,7 @@
   <dimension ref="A3:M171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -877,7 +871,7 @@
     </row>
     <row r="4" spans="4:9" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D4" s="12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1</v>
@@ -897,7 +891,7 @@
     </row>
     <row r="5" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D5" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E5" s="4">
         <v>44964</v>
@@ -915,7 +909,7 @@
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D6" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E6" s="4">
         <v>44965</v>
@@ -933,7 +927,7 @@
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D7" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E7" s="4">
         <v>44967</v>
@@ -951,7 +945,7 @@
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D8" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E8" s="4">
         <v>44970</v>
@@ -969,7 +963,7 @@
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D9" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E9" s="4">
         <v>44971</v>
@@ -989,7 +983,7 @@
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D10" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E10" s="4">
         <v>44972</v>
@@ -1007,7 +1001,7 @@
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D11" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E11" s="4">
         <v>44973</v>
@@ -1025,7 +1019,7 @@
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D12" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E12" s="4">
         <v>44974</v>
@@ -1045,7 +1039,7 @@
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D13" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E13" s="4">
         <v>44977</v>
@@ -1063,7 +1057,7 @@
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D14" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E14" s="4">
         <v>44978</v>
@@ -1081,7 +1075,7 @@
     </row>
     <row r="15" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D15" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E15" s="4">
         <v>44979</v>
@@ -1099,7 +1093,7 @@
     </row>
     <row r="16" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D16" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E16" s="4">
         <v>44981</v>
@@ -1117,7 +1111,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D17" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E17" s="4">
         <v>44984</v>
@@ -1135,7 +1129,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D18" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E18" s="4">
         <v>44985</v>
@@ -1144,7 +1138,7 @@
         <v>55</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>54</v>
@@ -1154,7 +1148,7 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="D19" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E19" s="4">
         <v>44987</v>
@@ -1163,16 +1157,16 @@
         <v>56</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D20" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E20" s="4">
         <v>44988</v>
@@ -1181,82 +1175,82 @@
         <v>57</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D21" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E21" s="4">
         <v>44992</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D22" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E22" s="4">
         <v>44993</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D23" s="6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E23" s="4">
         <v>44994</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D24" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E24" s="4">
         <v>44995</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="I24" s="3"/>
       <c r="M24" s="8" t="s">
@@ -1265,45 +1259,45 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D25" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E25" s="4">
         <v>44998</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="I25" s="3"/>
       <c r="M25" s="8"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D26" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E26" s="4">
         <v>44999</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I26" s="3"/>
       <c r="M26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D27" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E27" s="4">
         <v>45000</v>
@@ -1312,93 +1306,93 @@
         <v>58</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D28" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E28" s="4">
         <v>45001</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D29" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E29" s="4">
         <v>45002</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D30" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E30" s="4">
         <v>45006</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D31" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E31" s="4">
         <v>45007</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D32" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E32" s="4">
         <v>45008</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -1408,66 +1402,70 @@
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D33" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E33" s="4">
         <v>45009</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D34" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E34" s="6"/>
+        <v>108</v>
+      </c>
+      <c r="E34" s="4">
+        <v>45010</v>
+      </c>
       <c r="F34" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G34" s="10"/>
-      <c r="H34" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="I34" s="3"/>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D35" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="E35" s="4">
+        <v>45011</v>
+      </c>
+      <c r="F35" s="3"/>
       <c r="G35" s="10"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D36" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="E36" s="4">
+        <v>45012</v>
+      </c>
+      <c r="F36" s="3"/>
       <c r="G36" s="10"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D37" s="6" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E37" s="6"/>
-      <c r="F37" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="F37" s="3"/>
       <c r="G37" s="10"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -1475,9 +1473,7 @@
     <row r="38" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="F38" s="3"/>
       <c r="G38" s="10"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>

</xml_diff>

<commit_message>
Day-32 spring core with xml config
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\KTG\RAJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95B40BB-0E68-401E-9BF9-89E119F2FD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DDB71C-A04A-4B1E-84D3-F4EC5CD40FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="130">
   <si>
     <t>Concepts</t>
   </si>
@@ -410,6 +410,12 @@
   </si>
   <si>
     <t>refer spring core example</t>
+  </si>
+  <si>
+    <t>spring core setter and constructor injection autowiring</t>
+  </si>
+  <si>
+    <t>complete spring core with given examples</t>
   </si>
 </sst>
 </file>
@@ -852,7 +858,7 @@
   <dimension ref="A3:M171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1465,11 +1471,17 @@
         <v>110</v>
       </c>
       <c r="E36" s="4">
-        <v>45012</v>
-      </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="3"/>
+        <v>45015</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="I36" s="3"/>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.3">

</xml_diff>